<commit_message>
Not really sure what changed with the data here
</commit_message>
<xml_diff>
--- a/Practicum 1 Data.xlsx
+++ b/Practicum 1 Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b5d81501a8e5b23/Documents/Spring 2021/STAT-X 498/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b5d81501a8e5b23/Documents/Spring 2021/STAT-X 498/STAT-X 498 Practicum 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="25" documentId="11_CF9C1C55A61EBE21D1BF62A3FDCD25E883AA2257" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6ADD740E-BF56-4CF8-8CCD-82AEFB3A378E}"/>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:CE393"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CD10" sqref="CD10"/>
+      <selection activeCell="BZ7" sqref="BZ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Did early data cleaning. Still need to fix for loop so that only "No" values of weightgain end up having values of 0 for lbs_gained
</commit_message>
<xml_diff>
--- a/Practicum 1 Data.xlsx
+++ b/Practicum 1 Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b5d81501a8e5b23/Documents/Spring 2021/STAT-X 498/STAT-X 498 Practicum 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bilal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_CF9C1C55A61EBE21D1BF62A3FDCD25E883AA2257" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6ADD740E-BF56-4CF8-8CCD-82AEFB3A378E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DE9EDB-3CA6-4C37-AFAD-8A389EE24A29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:CE393"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BZ7" sqref="BZ7"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>